<commit_message>
Code Changes as part of RTI Scenario 7 Creation
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioTwo201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioTwo201718.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="53" activeTab="55"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1134,7 @@
     <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
@@ -4107,7 +4107,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7006,7 +7006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
@@ -7273,8 +7273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7347,8 +7347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Input file RTI Scenario 2 file checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioTwo201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioTwo201718.xlsx
@@ -1,80 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="11" activeTab="13"/>
+    <workbookView activeTab="13" firstSheet="11" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="15" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId10"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId11"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId12"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId13"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId14"/>
-    <sheet name="CreateLeaveRequest" sheetId="63" r:id="rId15"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="21" r:id="rId16"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId18"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId19"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="24" r:id="rId20"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId21"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId22"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId23"/>
-    <sheet name="UpdateLeaveRecord" sheetId="64" r:id="rId24"/>
-    <sheet name="CreateShPPLeaveRequest" sheetId="65" r:id="rId25"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="27" r:id="rId26"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId27"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId28"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId29"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="30" r:id="rId30"/>
-    <sheet name="UpdateLeaveRecord7" sheetId="66" r:id="rId31"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId32"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId33"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId34"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="33" r:id="rId35"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId36"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId37"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId38"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId39"/>
-    <sheet name="UpdateLeaveRecord9" sheetId="67" r:id="rId40"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId41"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId42"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId43"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId44"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId45"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId46"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId47"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="42" r:id="rId48"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId49"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId50"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId51"/>
-    <sheet name="ResetEmployeeData12" sheetId="62" r:id="rId52"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="45" r:id="rId53"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="46" r:id="rId54"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="60" r:id="rId55"/>
-    <sheet name="TestMarchReports" sheetId="47" r:id="rId56"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="15"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="18"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId11" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId12" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId13" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId14" sheetId="20"/>
+    <sheet name="CreateLeaveRequest" r:id="rId15" sheetId="63"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId16" sheetId="21"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId17" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId18" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId19" sheetId="23"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId20" sheetId="24"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId21" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId22" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId23" sheetId="26"/>
+    <sheet name="UpdateLeaveRecord" r:id="rId24" sheetId="64"/>
+    <sheet name="CreateShPPLeaveRequest" r:id="rId25" sheetId="65"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId26" sheetId="27"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId27" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId28" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId29" sheetId="29"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId30" sheetId="30"/>
+    <sheet name="UpdateLeaveRecord7" r:id="rId31" sheetId="66"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId32" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId33" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId34" sheetId="32"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId35" sheetId="33"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId36" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId37" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId38" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId39" sheetId="36"/>
+    <sheet name="UpdateLeaveRecord9" r:id="rId40" sheetId="67"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId41" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId42" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId43" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId44" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId45" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId46" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId47" sheetId="41"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId48" sheetId="42"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId49" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId50" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId51" sheetId="44"/>
+    <sheet name="ResetEmployeeData12" r:id="rId52" sheetId="62"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId53" sheetId="45"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId54" sheetId="46"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId55" sheetId="60"/>
+    <sheet name="TestMarchReports" r:id="rId56" sheetId="47"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="198">
   <si>
     <t>TC</t>
   </si>
@@ -675,6 +675,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -728,66 +729,66 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -804,10 +805,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -842,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -894,7 +895,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -999,7 +1000,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1008,13 +1009,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1024,7 +1025,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1033,7 +1034,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1042,7 +1043,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1052,12 +1053,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1088,7 +1089,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1107,7 +1108,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1119,7 +1120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
@@ -1128,10 +1129,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,12 +1934,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1947,22 +1948,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -2064,15 +2065,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2081,12 +2082,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2118,7 +2119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -2142,12 +2143,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2156,19 +2157,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2215,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -2255,14 +2256,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2271,13 +2272,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2324,7 +2325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -2364,14 +2365,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
@@ -2380,23 +2381,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5703125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -2498,14 +2499,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2514,18 +2515,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -2575,7 +2576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -2617,13 +2618,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2632,12 +2633,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2669,7 +2670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -2693,12 +2694,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2707,18 +2708,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2765,7 +2766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -2805,14 +2806,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2821,15 +2822,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2876,7 +2877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -2916,14 +2917,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2932,23 +2933,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -3050,14 +3051,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3066,10 +3067,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3095,7 +3096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -3118,13 +3119,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3133,13 +3134,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3171,7 +3172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -3195,12 +3196,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3209,18 +3210,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3267,7 +3268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -3307,14 +3308,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3323,13 +3324,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3376,7 +3377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -3416,14 +3417,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3432,23 +3433,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -3550,14 +3551,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3566,10 +3567,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3595,7 +3596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -3613,13 +3614,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3628,12 +3629,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3662,7 +3663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -3683,12 +3684,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3697,12 +3698,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3734,7 +3735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -3758,12 +3759,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3772,20 +3773,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3832,7 +3833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="65.45" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -3872,14 +3873,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3888,12 +3889,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3940,7 +3941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -3980,14 +3981,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3996,20 +3997,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -4062,7 +4063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -4111,14 +4112,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4127,10 +4128,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4162,7 +4163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -4186,13 +4187,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4201,12 +4202,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4238,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -4262,12 +4263,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4276,10 +4277,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4305,7 +4306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="2" s="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -4323,12 +4324,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4337,20 +4338,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4397,7 +4398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -4437,14 +4438,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4453,12 +4454,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4505,7 +4506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -4545,14 +4546,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4561,21 +4562,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -4628,7 +4629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -4677,14 +4678,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4693,12 +4694,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="51.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="51.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4730,7 +4731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -4754,12 +4755,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4768,18 +4769,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4826,7 +4827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -4866,14 +4867,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4882,12 +4883,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4934,7 +4935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -4974,14 +4975,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4990,21 +4991,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -5057,7 +5058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -5106,14 +5107,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5122,13 +5123,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5160,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -5184,12 +5185,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5198,18 +5199,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5256,7 +5257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -5296,15 +5297,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5313,10 +5314,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5342,7 +5343,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="2" s="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -5360,12 +5361,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5374,18 +5375,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5432,7 +5433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -5472,14 +5473,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5488,13 +5489,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="35.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5541,7 +5542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -5581,14 +5582,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5597,21 +5598,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -5664,7 +5665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -5713,14 +5714,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5729,12 +5730,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5766,7 +5767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -5790,12 +5791,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5804,18 +5805,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5862,7 +5863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -5902,14 +5903,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5918,12 +5919,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5970,7 +5971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6010,14 +6011,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6026,21 +6027,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -6093,7 +6094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6142,14 +6143,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6158,12 +6159,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6195,7 +6196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -6219,12 +6220,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6233,18 +6234,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6291,7 +6292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6331,14 +6332,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6347,18 +6348,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6405,7 +6406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6445,14 +6446,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6461,14 +6462,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6515,7 +6516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6555,14 +6556,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6571,20 +6572,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -6637,7 +6638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6686,14 +6687,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6702,8 +6703,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6723,7 +6724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>145</v>
       </c>
@@ -6737,13 +6738,13 @@
       <c r="E2" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6752,13 +6753,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6790,7 +6791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -6814,12 +6815,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6828,18 +6829,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6886,7 +6887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -6926,15 +6927,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6943,18 +6944,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7001,7 +7002,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -7041,15 +7042,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7058,20 +7059,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -7124,7 +7125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -7173,16 +7174,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -7191,23 +7192,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
@@ -7260,7 +7261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -7309,15 +7310,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7326,11 +7327,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7362,7 +7363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
@@ -7386,12 +7387,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7400,18 +7401,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7458,7 +7459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -7498,14 +7499,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7514,18 +7515,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7572,7 +7573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>195</v>
       </c>
@@ -7612,8 +7613,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>